<commit_message>
experiencias de complexidade terminadas
</commit_message>
<xml_diff>
--- a/report/minerals.xlsx
+++ b/report/minerals.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Angie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Angie/Documents/MIEIC/4A1S/AIAD/practice/project/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18860" yWindow="12520" windowWidth="26180" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="minerals" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="minerals 20" sheetId="4" r:id="rId5"/>
     <sheet name="minerals 25" sheetId="5" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -208,11 +211,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1693117872"/>
-        <c:axId val="1693119648"/>
+        <c:axId val="2049642752"/>
+        <c:axId val="2049820384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1693117872"/>
+        <c:axId val="2049642752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +228,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -238,7 +241,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>minerals</a:t>
                 </a:r>
               </a:p>
@@ -258,7 +261,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -296,7 +299,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -311,7 +314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1693119648"/>
+        <c:crossAx val="2049820384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -319,9 +322,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1693119648"/>
+        <c:axId val="2049820384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3500.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -346,7 +350,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -359,7 +363,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>tixks</a:t>
                 </a:r>
               </a:p>
@@ -379,7 +383,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -411,7 +415,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -426,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1693117872"/>
+        <c:crossAx val="2049642752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1035,16 +1039,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1063,7 +1067,164 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9588500" y="3556000"/>
+          <a:ext cx="6616700" cy="4470400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="size"/>
+      <sheetName val="size 10"/>
+      <sheetName val="size 20"/>
+      <sheetName val="size 30"/>
+      <sheetName val="size 40"/>
+      <sheetName val="size 50"/>
+      <sheetName val="size 60"/>
+      <sheetName val="size 70"/>
+      <sheetName val="size 80"/>
+      <sheetName val="size 90"/>
+      <sheetName val="size 100"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>ticks</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>10</v>
+          </cell>
+          <cell r="B2">
+            <v>374.2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>20</v>
+          </cell>
+          <cell r="B3">
+            <v>473.7</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>30</v>
+          </cell>
+          <cell r="B4">
+            <v>817.5</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>40</v>
+          </cell>
+          <cell r="B5">
+            <v>1157.5999999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>50</v>
+          </cell>
+          <cell r="B6">
+            <v>1756.7</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>60</v>
+          </cell>
+          <cell r="B7">
+            <v>2169</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>70</v>
+          </cell>
+          <cell r="B8">
+            <v>3052.6</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>80</v>
+          </cell>
+          <cell r="B9">
+            <v>3627.3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>90</v>
+          </cell>
+          <cell r="B10">
+            <v>4514.5</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>100</v>
+          </cell>
+          <cell r="B11">
+            <v>5809.6</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1331,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>